<commit_message>
Megcsinaltam a navigacios menut (lenyilo ablakok nelkul)
</commit_message>
<xml_diff>
--- a/Documentation/3 Portfólió projekt (Mobile first szemlélettel).xlsx
+++ b/Documentation/3 Portfólió projekt (Mobile first szemlélettel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Webfejlesztés\portfolio\work3\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906D9FB1-76E8-4442-9C5C-8AE36DDD045B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B420B8A4-6589-433A-B469-CDDBA9DDF427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D259B781-4274-4EB3-AA29-08B5222CEB9B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Git letöltése és beállítása vs code-hoz (első próbálkozás és a projekthez magához lokális repo).</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Betű típus beállítása h1..h6,p,span,button.</t>
+  </si>
+  <si>
+    <t>A képek és ikonok letöltése és rendszerezése.</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -444,7 +447,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +492,7 @@
       <c r="A5" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -502,10 +505,12 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">

</xml_diff>